<commit_message>
Add multiple scenario forecast notebooks
- Add three new forecast scenario notebooks:
  - 05: Optimistic scenario
  - 06: Normal scenario
  - 07: Conservative scenario
- Update Tesla scenarios Excel data file
</commit_message>
<xml_diff>
--- a/data/processed/Tesla_All_Sheets_Scenarios.xlsx
+++ b/data/processed/Tesla_All_Sheets_Scenarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LBKY\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tesla-optimus-business-analysis\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02E4A3-3A85-4E75-B672-7DDB38A613C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408FC60F-5875-46D6-973A-763A1EC97EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All_2030业务结构预测" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="CAGR_Analysis" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">All_各地区收入预测!$A$1:$D$190</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">All_传统业务预测!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">All_各地区收入预测!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="69">
   <si>
     <t>业务类型</t>
   </si>
@@ -98,12 +99,6 @@
     <t>年份</t>
   </si>
   <si>
-    <t>传统业务</t>
-  </si>
-  <si>
-    <t>新增业务</t>
-  </si>
-  <si>
     <t>YoY增长</t>
   </si>
   <si>
@@ -237,6 +232,15 @@
   </si>
   <si>
     <t>H_最终合并预测</t>
+  </si>
+  <si>
+    <t>总收入（亿美元）</t>
+  </si>
+  <si>
+    <t>新增业务（亿美元）</t>
+  </si>
+  <si>
+    <t>传统业务（亿美元）</t>
   </si>
 </sst>
 </file>
@@ -319,7 +323,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -341,6 +345,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="百分比" xfId="2" builtinId="5"/>
@@ -626,7 +631,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -652,7 +657,7 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="9">
         <v>1105.83</v>
       </c>
       <c r="D2" s="1">
@@ -666,7 +671,7 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="9">
         <v>698.13900000000001</v>
       </c>
       <c r="D3" s="1">
@@ -680,7 +685,7 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="9">
         <v>380.142</v>
       </c>
       <c r="D4" s="1">
@@ -694,7 +699,7 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="9">
         <v>270</v>
       </c>
       <c r="D5" s="1">
@@ -708,7 +713,7 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="9">
         <v>180</v>
       </c>
       <c r="D6" s="1">
@@ -722,7 +727,7 @@
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="9">
         <v>2634.1109999999999</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -736,7 +741,7 @@
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="9">
         <v>1413.0050000000001</v>
       </c>
       <c r="D8" s="1">
@@ -750,7 +755,7 @@
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="9">
         <v>892.06700000000001</v>
       </c>
       <c r="D9" s="1">
@@ -764,7 +769,7 @@
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="9">
         <v>485.73700000000002</v>
       </c>
       <c r="D10" s="1">
@@ -778,7 +783,7 @@
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="9">
         <v>345</v>
       </c>
       <c r="D11" s="1">
@@ -792,7 +797,7 @@
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="9">
         <v>230</v>
       </c>
       <c r="D12" s="1">
@@ -806,7 +811,7 @@
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="9">
         <v>3365.8090000000002</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -820,7 +825,7 @@
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="9">
         <v>1228.7</v>
       </c>
       <c r="D14" s="1">
@@ -834,7 +839,7 @@
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="9">
         <v>775.71</v>
       </c>
       <c r="D15" s="1">
@@ -848,7 +853,7 @@
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="9">
         <v>422.38</v>
       </c>
       <c r="D16" s="1">
@@ -862,7 +867,7 @@
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="9">
         <v>300</v>
       </c>
       <c r="D17" s="1">
@@ -876,7 +881,7 @@
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="9">
         <v>200</v>
       </c>
       <c r="D18" s="1">
@@ -890,7 +895,7 @@
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="9">
         <v>2926.79</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -907,10 +912,13 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="5" max="5" width="16.265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -920,556 +928,556 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="9">
         <v>814.62</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="9">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="9">
         <v>814.62</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="9">
         <v>967.73</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="9">
         <v>967.73</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="9">
         <v>976.9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="9">
         <v>0</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="9">
         <v>976.9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="9">
         <v>1077.25</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="9">
         <v>0</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="9">
         <v>1077.25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="9">
         <v>1230.53</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="9">
         <v>3</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="9">
         <v>1233.53</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="9">
         <v>1435.46</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="9">
         <v>25</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="9">
         <v>1460.46</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="9">
         <v>1691.25</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="9">
         <v>170</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="9">
         <v>1861.25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="9">
         <v>2014.25</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="9">
         <v>330</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="9">
         <v>2344.25</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="9">
         <v>2426.79</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="9">
         <v>500</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="9">
         <v>2926.79</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="9">
         <v>936.81299999999999</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="9">
         <v>0</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="9">
         <v>936.81299999999999</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="9">
         <v>1112.8895</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="9">
         <v>0</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="9">
         <v>1112.8895</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="9">
         <v>1123.4349999999999</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="9">
         <v>0</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="9">
         <v>1123.4349999999999</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="9">
         <v>1238.8375000000001</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="9">
         <v>0</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="9">
         <v>1238.8375000000001</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="9">
         <v>1415.1095</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="9">
         <v>3.45</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="9">
         <v>1418.5595000000001</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="9">
         <v>1650.779</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="9">
         <v>28.75</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="9">
         <v>1679.529</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="9">
         <v>1944.9375</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="9">
         <v>195.5</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="9">
         <v>2140.4375</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="9">
         <v>2316.3874999999998</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="9">
         <v>379.49999999999989</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="9">
         <v>2695.8874999999998</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="9">
         <v>2790.8085000000001</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="9">
         <v>575</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="9">
         <v>3365.8085000000001</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="9">
         <v>733.15800000000002</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="9">
         <v>0</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="9">
         <v>733.15800000000002</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="9">
         <v>870.95699999999999</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="9">
         <v>0</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="9">
         <v>870.95699999999999</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="9">
         <v>879.21</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="9">
         <v>0</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="9">
         <v>879.21</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="9">
         <v>969.52499999999998</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="9">
         <v>0</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="9">
         <v>969.52499999999998</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="9">
         <v>1107.4770000000001</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="9">
         <v>2.7</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="9">
         <v>1110.1769999999999</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="9">
         <v>1291.914</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="9">
         <v>22.5</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="9">
         <v>1314.414</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="9">
         <v>1522.125</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="9">
         <v>153</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="9">
         <v>1675.125</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="9">
         <v>1812.825</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="9">
         <v>297</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="9">
         <v>2109.8249999999998</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="9">
         <v>2184.1109999999999</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="9">
         <v>450</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="9">
         <v>2634.1109999999999</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1482,7 +1490,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1501,7 +1509,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -1811,11 +1819,11 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="3">
-        <v>2022</v>
+      <c r="A20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -1828,11 +1836,11 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="3">
-        <v>2023</v>
+      <c r="A21" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -1845,11 +1853,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" s="3">
-        <v>2024</v>
+      <c r="A22" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -1862,11 +1870,11 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" s="3">
-        <v>2025</v>
+      <c r="A23" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -1879,88 +1887,88 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" s="3">
-        <v>2026</v>
+      <c r="A24" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C24" s="3">
-        <v>3.45</v>
+        <v>2.7</v>
       </c>
       <c r="D24" s="3">
         <v>0</v>
       </c>
       <c r="E24" s="3">
-        <v>3.45</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="3">
-        <v>2027</v>
+      <c r="A25" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C25" s="3">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D25" s="3">
-        <v>5.75</v>
+        <v>4.5</v>
       </c>
       <c r="E25" s="3">
-        <v>28.75</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="3">
-        <v>2028</v>
+      <c r="A26" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C26" s="3">
-        <v>103.5</v>
+        <v>81</v>
       </c>
       <c r="D26" s="3">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="E26" s="3">
-        <v>195.5</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="3">
-        <v>2029</v>
+      <c r="A27" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C27" s="3">
-        <v>230</v>
+        <v>180</v>
       </c>
       <c r="D27" s="3">
-        <v>149.5</v>
+        <v>117</v>
       </c>
       <c r="E27" s="3">
-        <v>379.5</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="3">
-        <v>2030</v>
+      <c r="A28" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C28" s="3">
-        <v>345</v>
+        <v>270</v>
       </c>
       <c r="D28" s="3">
-        <v>230</v>
+        <v>180</v>
       </c>
       <c r="E28" s="3">
-        <v>575</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -1972,8 +1980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268A6313-443C-4907-BE89-2657B126D326}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1995,7 +2003,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -2005,16 +2013,16 @@
       <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="6">
         <v>714.62</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="6">
         <v>39.090000000000003</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="6">
         <v>60.91</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="6">
         <v>814.62</v>
       </c>
     </row>
@@ -2025,16 +2033,16 @@
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="6">
         <v>824.19</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
         <v>60.35</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="6">
         <v>83.19</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="6">
         <v>967.73</v>
       </c>
     </row>
@@ -2045,16 +2053,16 @@
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <v>770.7</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>100.86</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>105.34</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>976.9</v>
       </c>
     </row>
@@ -2065,16 +2073,16 @@
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="6">
         <v>800.02</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>144.22999999999999</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>133</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="6">
         <v>1077.25</v>
       </c>
     </row>
@@ -2085,16 +2093,16 @@
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>861.03</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>201.92</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>167.58</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>1230.53</v>
       </c>
     </row>
@@ -2105,16 +2113,16 @@
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="6">
         <v>941.62</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>282.69</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>211.15</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <v>1435.46</v>
       </c>
     </row>
@@ -2125,16 +2133,16 @@
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <v>1029.43</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>395.77</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>266.05</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
         <v>1691.25</v>
       </c>
     </row>
@@ -2145,16 +2153,16 @@
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <v>1124.95</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>554.08000000000004</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="6">
         <v>335.22</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="6">
         <v>2014.25</v>
       </c>
     </row>
@@ -2165,16 +2173,16 @@
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>1228.7</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>775.71</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="6">
         <v>422.38</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="6">
         <v>2426.79</v>
       </c>
     </row>
@@ -2185,16 +2193,16 @@
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="6">
         <v>821.81299999999999</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="6">
         <v>44.953499999999998</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="6">
         <v>70.046499999999995</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
         <v>936.81299999999999</v>
       </c>
     </row>
@@ -2205,16 +2213,16 @@
       <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="6">
         <v>947.81849999999997</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="6">
         <v>69.402500000000003</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="6">
         <v>95.668499999999995</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="6">
         <v>1112.8895</v>
       </c>
     </row>
@@ -2225,16 +2233,16 @@
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="6">
         <v>886.30499999999995</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="6">
         <v>115.989</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="6">
         <v>121.14100000000001</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="6">
         <v>1123.4349999999999</v>
       </c>
     </row>
@@ -2245,16 +2253,16 @@
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="6">
         <v>920.02300000000002</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
         <v>165.86449999999999</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="6">
         <v>152.94999999999999</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="6">
         <v>1238.8375000000001</v>
       </c>
     </row>
@@ -2265,16 +2273,16 @@
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="6">
         <v>990.18449999999996</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="6">
         <v>232.208</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="6">
         <v>192.71700000000001</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="6">
         <v>1415.1095</v>
       </c>
     </row>
@@ -2285,16 +2293,16 @@
       <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="6">
         <v>1082.8630000000001</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="6">
         <v>325.09350000000001</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="6">
         <v>242.82249999999999</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="6">
         <v>1650.779</v>
       </c>
     </row>
@@ -2305,16 +2313,16 @@
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="6">
         <v>1183.8444999999999</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="6">
         <v>455.13549999999998</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="6">
         <v>305.95749999999998</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="6">
         <v>1944.9375</v>
       </c>
     </row>
@@ -2325,16 +2333,16 @@
       <c r="B18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="6">
         <v>1293.6925000000001</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="6">
         <v>637.19200000000001</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="6">
         <v>385.50299999999999</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="6">
         <v>2316.3874999999998</v>
       </c>
     </row>
@@ -2345,200 +2353,201 @@
       <c r="B19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="6">
         <v>1413.0050000000001</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="6">
         <v>892.06650000000002</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="6">
         <v>485.73700000000002</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="6">
         <v>2790.8085000000001</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="3">
-        <v>2022</v>
+      <c r="A20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="3">
-        <v>821.81299999999999</v>
-      </c>
-      <c r="D20" s="3">
-        <v>44.953499999999998</v>
-      </c>
-      <c r="E20" s="3">
-        <v>70.046499999999995</v>
-      </c>
-      <c r="F20" s="3">
-        <v>936.81299999999999</v>
+        <v>5</v>
+      </c>
+      <c r="C20" s="6">
+        <v>643.15800000000002</v>
+      </c>
+      <c r="D20" s="6">
+        <v>35.180999999999997</v>
+      </c>
+      <c r="E20" s="6">
+        <v>54.819000000000003</v>
+      </c>
+      <c r="F20" s="6">
+        <v>733.15800000000002</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" s="3">
-        <v>2023</v>
+      <c r="A21" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="3">
-        <v>947.81849999999997</v>
-      </c>
-      <c r="D21" s="3">
-        <v>69.402500000000003</v>
-      </c>
-      <c r="E21" s="3">
-        <v>95.668499999999995</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1112.8895</v>
+        <v>5</v>
+      </c>
+      <c r="C21" s="6">
+        <v>741.77100000000007</v>
+      </c>
+      <c r="D21" s="6">
+        <v>54.314999999999998</v>
+      </c>
+      <c r="E21" s="6">
+        <v>74.870999999999995</v>
+      </c>
+      <c r="F21" s="6">
+        <v>870.95699999999999</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="3">
-        <v>2024</v>
+      <c r="A22" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="3">
-        <v>886.30499999999995</v>
-      </c>
-      <c r="D22" s="3">
-        <v>115.989</v>
-      </c>
-      <c r="E22" s="3">
-        <v>121.14100000000001</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1123.4349999999999</v>
+        <v>5</v>
+      </c>
+      <c r="C22" s="6">
+        <v>693.63000000000011</v>
+      </c>
+      <c r="D22" s="6">
+        <v>90.774000000000001</v>
+      </c>
+      <c r="E22" s="6">
+        <v>94.806000000000012</v>
+      </c>
+      <c r="F22" s="6">
+        <v>879.21</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="3">
-        <v>2025</v>
+      <c r="A23" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="3">
-        <v>920.02300000000002</v>
-      </c>
-      <c r="D23" s="3">
-        <v>165.86449999999999</v>
-      </c>
-      <c r="E23" s="3">
-        <v>152.94999999999999</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1238.8375000000001</v>
+        <v>5</v>
+      </c>
+      <c r="C23" s="6">
+        <v>720.01800000000003</v>
+      </c>
+      <c r="D23" s="6">
+        <v>129.80699999999999</v>
+      </c>
+      <c r="E23" s="6">
+        <v>119.7</v>
+      </c>
+      <c r="F23" s="6">
+        <v>969.52499999999998</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="3">
-        <v>2026</v>
+      <c r="A24" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="3">
-        <v>990.18449999999996</v>
-      </c>
-      <c r="D24" s="3">
-        <v>232.208</v>
-      </c>
-      <c r="E24" s="3">
-        <v>192.71700000000001</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1415.1095</v>
+        <v>5</v>
+      </c>
+      <c r="C24" s="6">
+        <v>774.92700000000002</v>
+      </c>
+      <c r="D24" s="6">
+        <v>181.72800000000001</v>
+      </c>
+      <c r="E24" s="6">
+        <v>150.822</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1107.4770000000001</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="3">
-        <v>2027</v>
+      <c r="A25" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1082.8630000000001</v>
-      </c>
-      <c r="D25" s="3">
-        <v>325.09350000000001</v>
-      </c>
-      <c r="E25" s="3">
-        <v>242.82249999999999</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1650.779</v>
+        <v>5</v>
+      </c>
+      <c r="C25" s="6">
+        <v>847.45799999999997</v>
+      </c>
+      <c r="D25" s="6">
+        <v>254.42099999999999</v>
+      </c>
+      <c r="E25" s="6">
+        <v>190.035</v>
+      </c>
+      <c r="F25" s="6">
+        <v>1291.914</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="3">
-        <v>2028</v>
+      <c r="A26" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="3">
-        <v>1183.8444999999999</v>
-      </c>
-      <c r="D26" s="3">
-        <v>455.13549999999998</v>
-      </c>
-      <c r="E26" s="3">
-        <v>305.95749999999998</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1944.9375</v>
+        <v>5</v>
+      </c>
+      <c r="C26" s="6">
+        <v>926.48700000000008</v>
+      </c>
+      <c r="D26" s="6">
+        <v>356.19299999999998</v>
+      </c>
+      <c r="E26" s="6">
+        <v>239.44499999999999</v>
+      </c>
+      <c r="F26" s="6">
+        <v>1522.125</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="3">
-        <v>2029</v>
+      <c r="A27" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="3">
-        <v>1293.6925000000001</v>
-      </c>
-      <c r="D27" s="3">
-        <v>637.19200000000001</v>
-      </c>
-      <c r="E27" s="3">
-        <v>385.50299999999999</v>
-      </c>
-      <c r="F27" s="3">
-        <v>2316.3874999999998</v>
+        <v>5</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1012.455</v>
+      </c>
+      <c r="D27" s="6">
+        <v>498.67200000000003</v>
+      </c>
+      <c r="E27" s="6">
+        <v>301.69799999999998</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1812.825</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="3">
-        <v>2030</v>
+      <c r="A28" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1413.0050000000001</v>
-      </c>
-      <c r="D28" s="3">
-        <v>892.06650000000002</v>
-      </c>
-      <c r="E28" s="3">
-        <v>485.73700000000002</v>
-      </c>
-      <c r="F28" s="3">
-        <v>2790.8085000000001</v>
+        <v>5</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1105.83</v>
+      </c>
+      <c r="D28" s="6">
+        <v>698.13900000000001</v>
+      </c>
+      <c r="E28" s="6">
+        <v>380.142</v>
+      </c>
+      <c r="F28" s="6">
+        <v>2184.1109999999999</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{268A6313-443C-4907-BE89-2657B126D326}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2548,7 +2557,7 @@
   <dimension ref="A1:H190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2564,10 +2573,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -2578,7 +2587,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6">
         <v>405.53</v>
@@ -2592,7 +2601,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="6">
         <v>452.8</v>
@@ -2606,7 +2615,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="6">
         <v>438</v>
@@ -2620,7 +2629,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="6">
         <v>486.04640000000018</v>
@@ -2634,7 +2643,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="6">
         <v>584.07848960000001</v>
@@ -2648,7 +2657,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="6">
         <v>745.7697529344</v>
@@ -2662,7 +2671,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="6">
         <v>1073.3419771222016</v>
@@ -2676,7 +2685,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="6">
         <v>1473.9851436580225</v>
@@ -2690,7 +2699,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="6">
         <v>1963.6573128521359</v>
@@ -2704,7 +2713,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11" s="6">
         <v>181.45</v>
@@ -2718,7 +2727,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="6">
         <v>251.01</v>
@@ -2732,7 +2741,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="6">
         <v>250.24</v>
@@ -2746,7 +2755,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="6">
         <v>267.76</v>
@@ -2760,7 +2769,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="6">
         <v>286.5</v>
@@ -2774,7 +2783,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16" s="6">
         <v>306.56</v>
@@ -2788,7 +2797,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="6">
         <v>328.02</v>
@@ -2802,7 +2811,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" s="6">
         <v>350.98</v>
@@ -2816,7 +2825,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19" s="6">
         <v>375.55</v>
@@ -2830,7 +2839,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D20" s="6">
         <v>80</v>
@@ -2844,7 +2853,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D21" s="6">
         <v>100.41</v>
@@ -2858,7 +2867,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" s="6">
         <v>104.26</v>
@@ -2872,7 +2881,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D23" s="6">
         <v>116.77</v>
@@ -2886,7 +2895,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="6">
         <v>130.78</v>
@@ -2900,7 +2909,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D25" s="6">
         <v>146.47</v>
@@ -2914,7 +2923,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D26" s="6">
         <v>164.05</v>
@@ -2928,7 +2937,7 @@
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D27" s="6">
         <v>183.74</v>
@@ -2942,7 +2951,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D28" s="6">
         <v>205.79</v>
@@ -2956,7 +2965,7 @@
         <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D29" s="6">
         <v>40</v>
@@ -2970,7 +2979,7 @@
         <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D30" s="6">
         <v>55.78</v>
@@ -2984,7 +2993,7 @@
         <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D31" s="6">
         <v>62.56</v>
@@ -2998,7 +3007,7 @@
         <v>14</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D32" s="6">
         <v>75.069999999999993</v>
@@ -3012,7 +3021,7 @@
         <v>14</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D33" s="6">
         <v>90.08</v>
@@ -3026,7 +3035,7 @@
         <v>14</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D34" s="6">
         <v>108.1</v>
@@ -3040,7 +3049,7 @@
         <v>14</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D35" s="6">
         <v>129.72</v>
@@ -3054,7 +3063,7 @@
         <v>14</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D36" s="6">
         <v>155.66</v>
@@ -3068,7 +3077,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D37" s="6">
         <v>186.79</v>
@@ -3082,7 +3091,7 @@
         <v>14</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D38" s="6">
         <v>15</v>
@@ -3096,7 +3105,7 @@
         <v>14</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D39" s="6">
         <v>20.079999999999998</v>
@@ -3110,7 +3119,7 @@
         <v>14</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D40" s="6">
         <v>20.85</v>
@@ -3124,7 +3133,7 @@
         <v>14</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D41" s="6">
         <v>23.98</v>
@@ -3138,7 +3147,7 @@
         <v>14</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D42" s="6">
         <v>27.58</v>
@@ -3152,7 +3161,7 @@
         <v>14</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D43" s="6">
         <v>31.72</v>
@@ -3166,7 +3175,7 @@
         <v>14</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D44" s="6">
         <v>36.479999999999997</v>
@@ -3180,7 +3189,7 @@
         <v>14</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D45" s="6">
         <v>41.95</v>
@@ -3194,7 +3203,7 @@
         <v>14</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D46" s="6">
         <v>48.24</v>
@@ -3208,7 +3217,7 @@
         <v>14</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D47" s="6">
         <v>92.64</v>
@@ -3222,7 +3231,7 @@
         <v>14</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D48" s="6">
         <v>87.82</v>
@@ -3236,7 +3245,7 @@
         <v>14</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D49" s="6">
         <v>101.15</v>
@@ -3250,7 +3259,7 @@
         <v>14</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D50" s="6">
         <v>107.62</v>
@@ -3264,7 +3273,7 @@
         <v>14</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D51" s="6">
         <v>114.51</v>
@@ -3278,7 +3287,7 @@
         <v>14</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D52" s="6">
         <v>121.84</v>
@@ -3292,7 +3301,7 @@
         <v>14</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D53" s="6">
         <v>129.63999999999999</v>
@@ -3306,7 +3315,7 @@
         <v>14</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D54" s="6">
         <v>137.94</v>
@@ -3320,7 +3329,7 @@
         <v>14</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D55" s="6">
         <v>146.77000000000001</v>
@@ -3334,7 +3343,7 @@
         <v>14</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D56" s="6">
         <v>814.62</v>
@@ -3348,7 +3357,7 @@
         <v>14</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D57" s="6">
         <v>967.73</v>
@@ -3362,7 +3371,7 @@
         <v>14</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D58" s="6">
         <v>976.9</v>
@@ -3376,7 +3385,7 @@
         <v>14</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D59" s="6">
         <v>1077.25</v>
@@ -3390,7 +3399,7 @@
         <v>14</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D60" s="6">
         <v>1233.5299999999997</v>
@@ -3404,7 +3413,7 @@
         <v>14</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D61" s="6">
         <v>1460.46</v>
@@ -3418,7 +3427,7 @@
         <v>14</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D62" s="6">
         <v>1861.25</v>
@@ -3432,7 +3441,7 @@
         <v>14</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D63" s="6">
         <v>2344.25</v>
@@ -3446,7 +3455,7 @@
         <v>14</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D64" s="6">
         <v>2926.79</v>
@@ -3460,7 +3469,7 @@
         <v>12</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D65" s="6">
         <v>405.53</v>
@@ -3474,7 +3483,7 @@
         <v>12</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D66" s="6">
         <v>452.8</v>
@@ -3488,7 +3497,7 @@
         <v>12</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D67" s="6">
         <v>438</v>
@@ -3502,7 +3511,7 @@
         <v>12</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D68" s="6">
         <v>558.95749999999998</v>
@@ -3517,7 +3526,7 @@
         <v>12</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D69" s="6">
         <v>671.69200000000001</v>
@@ -3532,7 +3541,7 @@
         <v>12</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D70" s="6">
         <v>857.63549999999987</v>
@@ -3547,7 +3556,7 @@
         <v>12</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D71" s="6">
         <v>1234.3409999999999</v>
@@ -3562,7 +3571,7 @@
         <v>12</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D72" s="6">
         <v>1695.0769999999998</v>
@@ -3577,7 +3586,7 @@
         <v>12</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D73" s="6">
         <v>2258.1975000000002</v>
@@ -3592,7 +3601,7 @@
         <v>12</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D74" s="6">
         <v>181.45</v>
@@ -3606,7 +3615,7 @@
         <v>12</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D75" s="6">
         <v>251.01</v>
@@ -3620,7 +3629,7 @@
         <v>12</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D76" s="6">
         <v>250.24</v>
@@ -3634,7 +3643,7 @@
         <v>12</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D77" s="6">
         <v>307.92399999999998</v>
@@ -3648,7 +3657,7 @@
         <v>12</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D78" s="6">
         <v>329.47500000000002</v>
@@ -3662,7 +3671,7 @@
         <v>12</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D79" s="6">
         <v>352.54399999999998</v>
@@ -3676,7 +3685,7 @@
         <v>12</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D80" s="6">
         <v>377.22300000000001</v>
@@ -3690,7 +3699,7 @@
         <v>12</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D81" s="6">
         <v>403.62700000000001</v>
@@ -3704,7 +3713,7 @@
         <v>12</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D82" s="6">
         <v>431.88249999999999</v>
@@ -3718,7 +3727,7 @@
         <v>12</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D83" s="6">
         <v>80</v>
@@ -3732,7 +3741,7 @@
         <v>12</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D84" s="6">
         <v>100.41</v>
@@ -3746,7 +3755,7 @@
         <v>12</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D85" s="6">
         <v>104.26</v>
@@ -3760,7 +3769,7 @@
         <v>12</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D86" s="6">
         <v>134.28550000000001</v>
@@ -3774,7 +3783,7 @@
         <v>12</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D87" s="6">
         <v>150.39699999999999</v>
@@ -3788,7 +3797,7 @@
         <v>12</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D88" s="6">
         <v>168.44049999999999</v>
@@ -3802,7 +3811,7 @@
         <v>12</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D89" s="6">
         <v>188.6575</v>
@@ -3816,7 +3825,7 @@
         <v>12</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D90" s="6">
         <v>211.30099999999999</v>
@@ -3830,7 +3839,7 @@
         <v>12</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D91" s="6">
         <v>236.6585</v>
@@ -3844,7 +3853,7 @@
         <v>12</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D92" s="6">
         <v>40</v>
@@ -3858,7 +3867,7 @@
         <v>12</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D93" s="6">
         <v>55.78</v>
@@ -3872,7 +3881,7 @@
         <v>12</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D94" s="6">
         <v>62.56</v>
@@ -3886,7 +3895,7 @@
         <v>12</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D95" s="6">
         <v>86.330500000000001</v>
@@ -3900,7 +3909,7 @@
         <v>12</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D96" s="6">
         <v>103.592</v>
@@ -3914,7 +3923,7 @@
         <v>12</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D97" s="6">
         <v>124.315</v>
@@ -3928,7 +3937,7 @@
         <v>12</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D98" s="6">
         <v>149.178</v>
@@ -3942,7 +3951,7 @@
         <v>12</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D99" s="6">
         <v>179.00899999999999</v>
@@ -3956,7 +3965,7 @@
         <v>12</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D100" s="6">
         <v>214.80850000000001</v>
@@ -3970,7 +3979,7 @@
         <v>12</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D101" s="6">
         <v>15</v>
@@ -3984,7 +3993,7 @@
         <v>12</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D102" s="6">
         <v>20.079999999999998</v>
@@ -3998,7 +4007,7 @@
         <v>12</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D103" s="6">
         <v>20.85</v>
@@ -4012,7 +4021,7 @@
         <v>12</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D104" s="6">
         <v>27.577000000000002</v>
@@ -4026,7 +4035,7 @@
         <v>12</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D105" s="6">
         <v>31.716999999999999</v>
@@ -4040,7 +4049,7 @@
         <v>12</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D106" s="6">
         <v>36.478000000000002</v>
@@ -4054,7 +4063,7 @@
         <v>12</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D107" s="6">
         <v>41.951999999999998</v>
@@ -4068,7 +4077,7 @@
         <v>12</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D108" s="6">
         <v>48.2425</v>
@@ -4082,7 +4091,7 @@
         <v>12</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D109" s="6">
         <v>55.475999999999999</v>
@@ -4096,7 +4105,7 @@
         <v>12</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D110" s="6">
         <v>92.64</v>
@@ -4110,7 +4119,7 @@
         <v>12</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D111" s="6">
         <v>87.82</v>
@@ -4124,7 +4133,7 @@
         <v>12</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D112" s="6">
         <v>101.15</v>
@@ -4138,7 +4147,7 @@
         <v>12</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D113" s="6">
         <v>123.76300000000001</v>
@@ -4152,7 +4161,7 @@
         <v>12</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D114" s="6">
         <v>131.6865</v>
@@ -4166,7 +4175,7 @@
         <v>12</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D115" s="6">
         <v>140.11600000000001</v>
@@ -4180,7 +4189,7 @@
         <v>12</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D116" s="6">
         <v>149.08600000000001</v>
@@ -4194,7 +4203,7 @@
         <v>12</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D117" s="6">
         <v>158.631</v>
@@ -4208,7 +4217,7 @@
         <v>12</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D118" s="6">
         <v>168.78550000000001</v>
@@ -4222,7 +4231,7 @@
         <v>12</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D119" s="6">
         <v>814.62</v>
@@ -4236,7 +4245,7 @@
         <v>12</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D120" s="6">
         <v>967.73</v>
@@ -4250,7 +4259,7 @@
         <v>12</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D121" s="6">
         <v>976.9</v>
@@ -4264,7 +4273,7 @@
         <v>12</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D122" s="6">
         <v>1238.8374999999999</v>
@@ -4278,7 +4287,7 @@
         <v>12</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D123" s="6">
         <v>1418.5595000000003</v>
@@ -4292,7 +4301,7 @@
         <v>12</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D124" s="6">
         <v>1679.5289999999998</v>
@@ -4306,7 +4315,7 @@
         <v>12</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D125" s="6">
         <v>2140.4375</v>
@@ -4320,7 +4329,7 @@
         <v>12</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D126" s="6">
         <v>2695.8874999999994</v>
@@ -4334,7 +4343,7 @@
         <v>12</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D127" s="6">
         <v>3365.8085000000005</v>
@@ -4348,7 +4357,7 @@
         <v>5</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D128" s="6">
         <v>405.53</v>
@@ -4362,7 +4371,7 @@
         <v>5</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D129" s="6">
         <v>452.8</v>
@@ -4376,7 +4385,7 @@
         <v>5</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D130" s="6">
         <v>438</v>
@@ -4390,7 +4399,7 @@
         <v>5</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D131" s="6">
         <v>437.44499999999999</v>
@@ -4405,7 +4414,7 @@
         <v>5</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D132" s="6">
         <v>525.67199999999991</v>
@@ -4420,7 +4429,7 @@
         <v>5</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D133" s="6">
         <v>671.19299999999998</v>
@@ -4435,7 +4444,7 @@
         <v>5</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D134" s="6">
         <v>966.00600000000009</v>
@@ -4450,7 +4459,7 @@
         <v>5</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D135" s="6">
         <v>1326.5819999999999</v>
@@ -4465,7 +4474,7 @@
         <v>5</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D136" s="6">
         <v>1767.2849999999999</v>
@@ -4480,7 +4489,7 @@
         <v>5</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D137" s="6">
         <v>181.45</v>
@@ -4494,7 +4503,7 @@
         <v>5</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D138" s="6">
         <v>251.01</v>
@@ -4508,7 +4517,7 @@
         <v>5</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D139" s="6">
         <v>250.24</v>
@@ -4522,7 +4531,7 @@
         <v>5</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D140" s="6">
         <v>240.98400000000001</v>
@@ -4536,7 +4545,7 @@
         <v>5</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D141" s="6">
         <v>257.85000000000002</v>
@@ -4550,7 +4559,7 @@
         <v>5</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D142" s="6">
         <v>275.904</v>
@@ -4564,7 +4573,7 @@
         <v>5</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D143" s="6">
         <v>295.21800000000002</v>
@@ -4578,7 +4587,7 @@
         <v>5</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D144" s="6">
         <v>315.88200000000001</v>
@@ -4592,7 +4601,7 @@
         <v>5</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D145" s="6">
         <v>337.995</v>
@@ -4606,7 +4615,7 @@
         <v>5</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D146" s="6">
         <v>80</v>
@@ -4620,7 +4629,7 @@
         <v>5</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D147" s="6">
         <v>100.41</v>
@@ -4634,7 +4643,7 @@
         <v>5</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D148" s="6">
         <v>104.26</v>
@@ -4648,7 +4657,7 @@
         <v>5</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D149" s="6">
         <v>105.093</v>
@@ -4662,7 +4671,7 @@
         <v>5</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D150" s="6">
         <v>117.702</v>
@@ -4676,7 +4685,7 @@
         <v>5</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D151" s="6">
         <v>131.82300000000001</v>
@@ -4690,7 +4699,7 @@
         <v>5</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D152" s="6">
         <v>147.64500000000001</v>
@@ -4704,7 +4713,7 @@
         <v>5</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D153" s="6">
         <v>165.36600000000001</v>
@@ -4718,7 +4727,7 @@
         <v>5</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D154" s="6">
         <v>185.21100000000001</v>
@@ -4732,7 +4741,7 @@
         <v>5</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D155" s="6">
         <v>40</v>
@@ -4746,7 +4755,7 @@
         <v>5</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D156" s="6">
         <v>55.78</v>
@@ -4760,7 +4769,7 @@
         <v>5</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D157" s="6">
         <v>62.56</v>
@@ -4774,7 +4783,7 @@
         <v>5</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D158" s="6">
         <v>67.563000000000002</v>
@@ -4788,7 +4797,7 @@
         <v>5</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D159" s="6">
         <v>81.072000000000003</v>
@@ -4802,7 +4811,7 @@
         <v>5</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D160" s="6">
         <v>97.29</v>
@@ -4816,7 +4825,7 @@
         <v>5</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D161" s="6">
         <v>116.748</v>
@@ -4830,7 +4839,7 @@
         <v>5</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D162" s="6">
         <v>140.09399999999999</v>
@@ -4844,7 +4853,7 @@
         <v>5</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D163" s="6">
         <v>168.11099999999999</v>
@@ -4858,7 +4867,7 @@
         <v>5</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D164" s="6">
         <v>15</v>
@@ -4872,7 +4881,7 @@
         <v>5</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D165" s="6">
         <v>20.079999999999998</v>
@@ -4886,7 +4895,7 @@
         <v>5</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D166" s="6">
         <v>20.85</v>
@@ -4900,7 +4909,7 @@
         <v>5</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D167" s="6">
         <v>21.582000000000001</v>
@@ -4914,7 +4923,7 @@
         <v>5</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D168" s="6">
         <v>24.821999999999999</v>
@@ -4928,7 +4937,7 @@
         <v>5</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D169" s="6">
         <v>28.547999999999998</v>
@@ -4942,7 +4951,7 @@
         <v>5</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D170" s="6">
         <v>32.832000000000001</v>
@@ -4956,7 +4965,7 @@
         <v>5</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D171" s="6">
         <v>37.755000000000003</v>
@@ -4970,7 +4979,7 @@
         <v>5</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D172" s="6">
         <v>43.415999999999997</v>
@@ -4984,7 +4993,7 @@
         <v>5</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D173" s="6">
         <v>92.64</v>
@@ -4998,7 +5007,7 @@
         <v>5</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D174" s="6">
         <v>87.82</v>
@@ -5012,7 +5021,7 @@
         <v>5</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D175" s="6">
         <v>101.15</v>
@@ -5026,7 +5035,7 @@
         <v>5</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D176" s="6">
         <v>96.858000000000004</v>
@@ -5040,7 +5049,7 @@
         <v>5</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D177" s="6">
         <v>103.059</v>
@@ -5054,7 +5063,7 @@
         <v>5</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D178" s="6">
         <v>109.65600000000001</v>
@@ -5068,7 +5077,7 @@
         <v>5</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D179" s="6">
         <v>116.676</v>
@@ -5082,7 +5091,7 @@
         <v>5</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D180" s="6">
         <v>124.146</v>
@@ -5096,7 +5105,7 @@
         <v>5</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D181" s="6">
         <v>132.09299999999999</v>
@@ -5110,7 +5119,7 @@
         <v>5</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D182" s="6">
         <v>814.62</v>
@@ -5124,7 +5133,7 @@
         <v>5</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D183" s="6">
         <v>967.73</v>
@@ -5138,7 +5147,7 @@
         <v>5</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D184" s="6">
         <v>976.9</v>
@@ -5152,7 +5161,7 @@
         <v>5</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D185" s="6">
         <v>969.52499999999986</v>
@@ -5166,7 +5175,7 @@
         <v>5</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D186" s="6">
         <v>1110.1769999999999</v>
@@ -5180,7 +5189,7 @@
         <v>5</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D187" s="6">
         <v>1314.414</v>
@@ -5194,7 +5203,7 @@
         <v>5</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D188" s="6">
         <v>1675.1250000000002</v>
@@ -5208,7 +5217,7 @@
         <v>5</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D189" s="6">
         <v>2109.8250000000003</v>
@@ -5222,13 +5231,14 @@
         <v>5</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D190" s="6">
         <v>2634.1109999999999</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{C80B7E88-3108-42CC-B320-CF1832D9B49A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5237,8 +5247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5D4D1B-3ECE-4B68-A9F7-9A991FBE60F5}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5248,45 +5258,45 @@
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" s="8">
         <f>(H2/F2)^(1/6)-1</f>
@@ -5315,13 +5325,13 @@
     </row>
     <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="8">
         <f t="shared" ref="D3:D7" si="0">(H3/F3)^(1/6)-1</f>
@@ -5350,13 +5360,13 @@
     </row>
     <row r="4" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="0"/>
@@ -5385,13 +5395,13 @@
     </row>
     <row r="5" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" si="0"/>
@@ -5418,13 +5428,13 @@
     </row>
     <row r="6" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="0"/>
@@ -5451,13 +5461,13 @@
     </row>
     <row r="7" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="0"/>
@@ -5484,13 +5494,13 @@
     </row>
     <row r="8" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D8" s="8">
         <f>(H8/F8)^(1/3)-1</f>
@@ -5517,13 +5527,13 @@
     </row>
     <row r="9" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" ref="D9:D10" si="3">(H9/F9)^(1/3)-1</f>
@@ -5550,13 +5560,13 @@
     </row>
     <row r="10" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D10" s="8">
         <f t="shared" si="3"/>
@@ -5583,13 +5593,13 @@
     </row>
     <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11" s="8">
         <v>1.1797699419232957</v>
@@ -5615,13 +5625,13 @@
     </row>
     <row r="12" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D12" s="8">
         <v>1.2289660400275799</v>
@@ -5647,13 +5657,13 @@
     </row>
     <row r="13" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" s="8">
         <v>1.2006697678186509</v>

</xml_diff>